<commit_message>
Fixed excel column width
</commit_message>
<xml_diff>
--- a/outputFiles/konkurser-2023-02-01.xlsx
+++ b/outputFiles/konkurser-2023-02-01.xlsx
@@ -401,6 +401,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">

</xml_diff>